<commit_message>
Fixing create/edit function in dealers, adding admin abilitiy to see all onderhouds
</commit_message>
<xml_diff>
--- a/docs/Tijdsverantwoordingen/TV Roman.xlsx
+++ b/docs/Tijdsverantwoordingen/TV Roman.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Documents\Github\MVC-Project-S4-Groep-4\docs\Tijdsverantwoordingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1772253-999A-42B3-8CD5-AB3D3E95BE21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB25AE1-23FA-4C1B-966C-E7B22156F4F9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6000" xr2:uid="{A1E42A40-59B0-438B-BBE0-97FEB3D675FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Taak</t>
   </si>
@@ -61,15 +61,20 @@
   </si>
   <si>
     <t>Technisch ontwerp</t>
+  </si>
+  <si>
+    <t>Realiseren programma</t>
+  </si>
+  <si>
+    <t>11-06 / 17-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -168,12 +173,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -496,7 +499,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,107 +512,120 @@
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
-        <v>1.3888888888888889E-3</v>
+      <c r="C3" s="6">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="6">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="6">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1.4583333333333333</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="4"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="4"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="4"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="4"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="4"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="1"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="1"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="6">
         <f>SUM(C2:C15)</f>
-        <v>0.48055555555555551</v>
+        <v>2.125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>